<commit_message>
commented spring security and added book component
</commit_message>
<xml_diff>
--- a/book_project/Book_Data.xlsx
+++ b/book_project/Book_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Id</t>
   </si>
@@ -52,6 +52,36 @@
   </si>
   <si>
     <t>SWT_Book</t>
+  </si>
+  <si>
+    <t>Ram_Book</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>Java_Book</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Python_Book</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Angular_Book</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>React_book</t>
+  </si>
+  <si>
+    <t>React</t>
   </si>
 </sst>
 </file>
@@ -390,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +499,76 @@
         <v>10</v>
       </c>
       <c r="D5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
         <v>5000</v>
       </c>
     </row>

</xml_diff>